<commit_message>
Update particular row, add new row
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,338 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nodejs Excel work\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D20063-E9F4-4AC4-8C0D-09587B338807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="98">
-  <si>
-    <t>phoneNumber</t>
-  </si>
-  <si>
-    <t>fullName</t>
-  </si>
-  <si>
-    <t>aum</t>
-  </si>
-  <si>
-    <t>08 Jun 2023</t>
-  </si>
-  <si>
-    <t>09 Jun 2023</t>
-  </si>
-  <si>
-    <t>10 Jun 2023</t>
-  </si>
-  <si>
-    <t>11 Jun 2023</t>
-  </si>
-  <si>
-    <t>12 Jun 2023</t>
-  </si>
-  <si>
-    <t>13 Jun 2023</t>
-  </si>
-  <si>
-    <t>14 Jun 2023</t>
-  </si>
-  <si>
-    <t>15 Jun 2023</t>
-  </si>
-  <si>
-    <t>16 Jun 2023</t>
-  </si>
-  <si>
-    <t>17 Jun 2023</t>
-  </si>
-  <si>
-    <t>18 Jun 2023</t>
-  </si>
-  <si>
-    <t>19 Jun 2023</t>
-  </si>
-  <si>
-    <t>20 Jun 2023</t>
-  </si>
-  <si>
-    <t>21 Jun 2023</t>
-  </si>
-  <si>
-    <t>22 Jun 2023</t>
-  </si>
-  <si>
-    <t>23 Jun 2023</t>
-  </si>
-  <si>
-    <t>24 Jun 2023</t>
-  </si>
-  <si>
-    <t>25 Jun 2023</t>
-  </si>
-  <si>
-    <t>26 Jun 2023</t>
-  </si>
-  <si>
-    <t>27 Jun 2023</t>
-  </si>
-  <si>
-    <t>28 Jun 2023</t>
-  </si>
-  <si>
-    <t>29 Jun 2023</t>
-  </si>
-  <si>
-    <t>30 Jun 2023</t>
-  </si>
-  <si>
-    <t>03162248589</t>
-  </si>
-  <si>
-    <t>Hassan Mehmood</t>
-  </si>
-  <si>
-    <t>137501.19</t>
-  </si>
-  <si>
-    <t>01234567890</t>
-  </si>
-  <si>
-    <t>test aqib</t>
-  </si>
-  <si>
-    <t>12366.73</t>
-  </si>
-  <si>
-    <t>03350250690</t>
-  </si>
-  <si>
-    <t>Syed Affan Aslam</t>
-  </si>
-  <si>
-    <t>258138.40</t>
-  </si>
-  <si>
-    <t>03482173757</t>
-  </si>
-  <si>
-    <t>Farhan Nadeem</t>
-  </si>
-  <si>
-    <t>50322.00</t>
-  </si>
-  <si>
-    <t>03349026073</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shahryar  test </t>
-  </si>
-  <si>
-    <t>5443.50</t>
-  </si>
-  <si>
-    <t>03363864574</t>
-  </si>
-  <si>
-    <t>Muhammad Asad</t>
-  </si>
-  <si>
-    <t>943.50</t>
-  </si>
-  <si>
-    <t>04528763916</t>
-  </si>
-  <si>
-    <t>test  user</t>
-  </si>
-  <si>
-    <t>7479.50</t>
-  </si>
-  <si>
-    <t>01234567899</t>
-  </si>
-  <si>
-    <t>Far nad</t>
-  </si>
-  <si>
-    <t>27345.56</t>
-  </si>
-  <si>
-    <t>03205425000</t>
-  </si>
-  <si>
-    <t>test twst</t>
-  </si>
-  <si>
-    <t>10864.70</t>
-  </si>
-  <si>
-    <t>03545878788</t>
-  </si>
-  <si>
-    <t>test test</t>
-  </si>
-  <si>
-    <t>22276.00</t>
-  </si>
-  <si>
-    <t>06467648154</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hassan Mehmood </t>
-  </si>
-  <si>
-    <t>5662.00</t>
-  </si>
-  <si>
-    <t>03564648498</t>
-  </si>
-  <si>
-    <t>Hassan Test</t>
-  </si>
-  <si>
-    <t>9305.00</t>
-  </si>
-  <si>
-    <t>03164656565</t>
-  </si>
-  <si>
-    <t>hassan Mehmood  tesy</t>
-  </si>
-  <si>
-    <t>3308.00</t>
-  </si>
-  <si>
-    <t>06424643535</t>
-  </si>
-  <si>
-    <t>new tesy</t>
-  </si>
-  <si>
-    <t>3772.00</t>
-  </si>
-  <si>
-    <t>06535356226</t>
-  </si>
-  <si>
-    <t>987.00</t>
-  </si>
-  <si>
-    <t>06535335326</t>
-  </si>
-  <si>
-    <t>hassan test</t>
-  </si>
-  <si>
-    <t>99.90</t>
-  </si>
-  <si>
-    <t>03699949498</t>
-  </si>
-  <si>
-    <t>Hassan yesy</t>
-  </si>
-  <si>
-    <t>3043.00</t>
-  </si>
-  <si>
-    <t>03464540151</t>
-  </si>
-  <si>
-    <t>Hassssan Test</t>
-  </si>
-  <si>
-    <t>37008.00</t>
-  </si>
-  <si>
-    <t>03333335599</t>
-  </si>
-  <si>
-    <t xml:space="preserve">restrict  pot </t>
-  </si>
-  <si>
-    <t>8730.50</t>
-  </si>
-  <si>
-    <t>03326299959</t>
-  </si>
-  <si>
-    <t>alfalaah test</t>
-  </si>
-  <si>
-    <t>03564988457</t>
-  </si>
-  <si>
-    <t>test tsst</t>
-  </si>
-  <si>
-    <t>6798.00</t>
-  </si>
-  <si>
-    <t>03464688000</t>
-  </si>
-  <si>
-    <t>yshsj hsyshs</t>
-  </si>
-  <si>
-    <t>2369.00</t>
-  </si>
-  <si>
-    <t>06735316616</t>
-  </si>
-  <si>
-    <t>test khan</t>
-  </si>
-  <si>
-    <t>1168.50</t>
-  </si>
-  <si>
-    <t>07789351713</t>
-  </si>
-  <si>
-    <t>mariam hasa</t>
-  </si>
-  <si>
-    <t>49875.70</t>
-  </si>
-  <si>
-    <t>Net movement in 30 days</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Incentive </t>
-  </si>
-</sst>
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -361,23 +64,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -702,127 +396,117 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AB44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
-    </sheetView>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="26" width="15" customWidth="1"/>
-    <col min="27" max="27" width="22.59765625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>phoneNumber</v>
+      </c>
+      <c r="B1" t="str">
+        <v>fullName</v>
+      </c>
+      <c r="C1" t="str">
+        <v>aum</v>
+      </c>
+      <c r="D1" t="str">
+        <v>code</v>
+      </c>
+      <c r="E1" t="str">
+        <v>08 Jun 2023</v>
+      </c>
+      <c r="F1" t="str">
+        <v>09 Jun 2023</v>
+      </c>
+      <c r="G1" t="str">
+        <v>10 Jun 2023</v>
+      </c>
+      <c r="H1" t="str">
+        <v>11 Jun 2023</v>
+      </c>
+      <c r="I1" t="str">
+        <v>12 Jun 2023</v>
+      </c>
+      <c r="J1" t="str">
+        <v>13 Jun 2023</v>
+      </c>
+      <c r="K1" t="str">
+        <v>14 Jun 2023</v>
+      </c>
+      <c r="L1" t="str">
+        <v>15 Jun 2023</v>
+      </c>
+      <c r="M1" t="str">
+        <v>16 Jun 2023</v>
+      </c>
+      <c r="N1" t="str">
+        <v>17 Jun 2023</v>
+      </c>
+      <c r="O1" t="str">
+        <v>18 Jun 2023</v>
+      </c>
+      <c r="P1" t="str">
+        <v>19 Jun 2023</v>
+      </c>
+      <c r="Q1" t="str">
+        <v>20 Jun 2023</v>
+      </c>
+      <c r="R1" t="str">
+        <v>21 Jun 2023</v>
+      </c>
+      <c r="S1" t="str">
+        <v>22 Jun 2023</v>
+      </c>
+      <c r="T1" t="str">
+        <v>23 Jun 2023</v>
+      </c>
+      <c r="U1" t="str">
+        <v>24 Jun 2023</v>
+      </c>
+      <c r="V1" t="str">
+        <v>25 Jun 2023</v>
+      </c>
+      <c r="W1" t="str">
+        <v>26 Jun 2023</v>
+      </c>
+      <c r="X1" t="str">
+        <v>27 Jun 2023</v>
+      </c>
+      <c r="Y1" t="str">
+        <v>28 Jun 2023</v>
+      </c>
+      <c r="Z1" t="str">
+        <v>29 Jun 2023</v>
+      </c>
+      <c r="AA1" t="str">
+        <v>30 Jun 2023</v>
+      </c>
+      <c r="AB1" t="str">
+        <v>Net movement in 30 days</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>03162248589</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Hassan Mehmood</v>
+      </c>
+      <c r="C2" t="str">
+        <v>137501.19</v>
+      </c>
+      <c r="D2" t="str">
+        <v>AC-1</v>
       </c>
       <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
         <v>1200</v>
       </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
       <c r="G2">
         <v>0</v>
       </c>
@@ -884,26 +568,25 @@
         <v>0</v>
       </c>
       <c r="AA2">
-        <f>SUM(D2:Z2)</f>
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <f>SUM(E2:AA2)</f>
         <v>1200</v>
       </c>
-      <c r="AB2">
-        <f>+AA2*0.5%</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>01234567890</v>
+      </c>
+      <c r="B3" t="str">
+        <v>test aqib</v>
+      </c>
+      <c r="C3" t="str">
+        <v>12366.73</v>
+      </c>
+      <c r="D3" t="str">
+        <v>AC-1</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -972,26 +655,25 @@
         <v>0</v>
       </c>
       <c r="AA3">
-        <f t="shared" ref="AA3:AA25" si="0">SUM(D3:Z3)</f>
         <v>0</v>
       </c>
       <c r="AB3">
-        <f t="shared" ref="AB3:AB25" si="1">+AA3*0.5%</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
+        <f>SUM(E3:AA3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>03350250690</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Syed Affan Aslam</v>
+      </c>
+      <c r="C4" t="str">
+        <v>258138.40</v>
+      </c>
+      <c r="D4" t="str">
+        <v>AC-1</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -1060,26 +742,25 @@
         <v>0</v>
       </c>
       <c r="AA4">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
+        <f>SUM(E4:AA4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>03482173757</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Farhan Nadeem</v>
+      </c>
+      <c r="C5" t="str">
+        <v>50322.00</v>
+      </c>
+      <c r="D5" t="str">
+        <v>AC-1</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -1148,26 +829,25 @@
         <v>0</v>
       </c>
       <c r="AA5">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
+        <f>SUM(E5:AA5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>03349026073</v>
+      </c>
+      <c r="B6" t="str">
+        <v xml:space="preserve">shahryar  test </v>
+      </c>
+      <c r="C6" t="str">
+        <v>5443.50</v>
+      </c>
+      <c r="D6" t="str">
+        <v>AC-1</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -1236,26 +916,25 @@
         <v>0</v>
       </c>
       <c r="AA6">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
+        <f>SUM(E6:AA6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>03363864574</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Muhammad Asad</v>
+      </c>
+      <c r="C7" t="str">
+        <v>943.50</v>
+      </c>
+      <c r="D7" t="str">
+        <v>AC-1</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -1324,26 +1003,25 @@
         <v>0</v>
       </c>
       <c r="AA7">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
+        <f>SUM(E7:AA7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>04528763916</v>
+      </c>
+      <c r="B8" t="str">
+        <v>test  user</v>
+      </c>
+      <c r="C8" t="str">
+        <v>7479.50</v>
+      </c>
+      <c r="D8" t="str">
+        <v>AC-1</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -1412,26 +1090,25 @@
         <v>0</v>
       </c>
       <c r="AA8">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
+        <f>SUM(E8:AA8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>01234567899</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Far nad</v>
+      </c>
+      <c r="C9" t="str">
+        <v>27345.56</v>
+      </c>
+      <c r="D9" t="str">
+        <v>AC-1</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -1500,26 +1177,25 @@
         <v>0</v>
       </c>
       <c r="AA9">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
+        <f>SUM(E9:AA9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>03205425000</v>
+      </c>
+      <c r="B10" t="str">
+        <v>test twst</v>
+      </c>
+      <c r="C10" t="str">
+        <v>10864.70</v>
+      </c>
+      <c r="D10" t="str">
+        <v>AC-1</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -1588,26 +1264,25 @@
         <v>0</v>
       </c>
       <c r="AA10">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B11" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
+        <f>SUM(E10:AA10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>03545878788</v>
+      </c>
+      <c r="B11" t="str">
+        <v>test test</v>
+      </c>
+      <c r="C11" t="str">
+        <v>22276.00</v>
+      </c>
+      <c r="D11" t="str">
+        <v>AC-1</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -1676,30 +1351,29 @@
         <v>0</v>
       </c>
       <c r="AA11">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>56</v>
-      </c>
-      <c r="B12" t="s">
-        <v>57</v>
-      </c>
-      <c r="C12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12">
+        <f>SUM(E11:AA11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>06467648154</v>
+      </c>
+      <c r="B12" t="str">
+        <v xml:space="preserve">hassan Mehmood </v>
+      </c>
+      <c r="C12" t="str">
+        <v>5662.00</v>
+      </c>
+      <c r="D12" t="str">
+        <v>AC-1</v>
+      </c>
+      <c r="E12">
         <v>52000</v>
       </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
       <c r="F12">
         <v>0</v>
       </c>
@@ -1764,26 +1438,25 @@
         <v>0</v>
       </c>
       <c r="AA12">
-        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AB12">
+        <f>SUM(E12:AA12)</f>
         <v>52000</v>
       </c>
-      <c r="AB12">
-        <f t="shared" si="1"/>
-        <v>260</v>
-      </c>
-    </row>
-    <row r="13" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>59</v>
-      </c>
-      <c r="B13" t="s">
-        <v>60</v>
-      </c>
-      <c r="C13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>03564648498</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Hassan Test</v>
+      </c>
+      <c r="C13" t="str">
+        <v>9305.00</v>
+      </c>
+      <c r="D13" t="str">
+        <v>AC-1</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -1852,26 +1525,25 @@
         <v>0</v>
       </c>
       <c r="AA13">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>62</v>
-      </c>
-      <c r="B14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14" t="s">
-        <v>64</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
+        <f>SUM(E13:AA13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>03164656565</v>
+      </c>
+      <c r="B14" t="str">
+        <v>hassan Mehmood  tesy</v>
+      </c>
+      <c r="C14" t="str">
+        <v>3308.00</v>
+      </c>
+      <c r="D14" t="str">
+        <v>AC-1</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -1940,26 +1612,25 @@
         <v>0</v>
       </c>
       <c r="AA14">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>65</v>
-      </c>
-      <c r="B15" t="s">
-        <v>66</v>
-      </c>
-      <c r="C15" t="s">
-        <v>67</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
+        <f>SUM(E14:AA14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>06424643535</v>
+      </c>
+      <c r="B15" t="str">
+        <v>new tesy</v>
+      </c>
+      <c r="C15" t="str">
+        <v>3772.00</v>
+      </c>
+      <c r="D15" t="str">
+        <v>AC-1</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -2028,26 +1699,25 @@
         <v>0</v>
       </c>
       <c r="AA15">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>68</v>
-      </c>
-      <c r="B16" t="s">
-        <v>66</v>
-      </c>
-      <c r="C16" t="s">
-        <v>69</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
+        <f>SUM(E15:AA15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>06535356226</v>
+      </c>
+      <c r="B16" t="str">
+        <v>new tesy</v>
+      </c>
+      <c r="C16" t="str">
+        <v>987.00</v>
+      </c>
+      <c r="D16" t="str">
+        <v>AC-1</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -2116,26 +1786,25 @@
         <v>0</v>
       </c>
       <c r="AA16">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>70</v>
-      </c>
-      <c r="B17" t="s">
-        <v>71</v>
-      </c>
-      <c r="C17" t="s">
-        <v>72</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
+        <f>SUM(E16:AA16)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>06535335326</v>
+      </c>
+      <c r="B17" t="str">
+        <v>hassan test</v>
+      </c>
+      <c r="C17" t="str">
+        <v>99.90</v>
+      </c>
+      <c r="D17" t="str">
+        <v>AC-1</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -2204,26 +1873,25 @@
         <v>0</v>
       </c>
       <c r="AA17">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>73</v>
-      </c>
-      <c r="B18" t="s">
-        <v>74</v>
-      </c>
-      <c r="C18" t="s">
-        <v>75</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
+        <f>SUM(E17:AA17)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>03699949498</v>
+      </c>
+      <c r="B18" t="str">
+        <v>Hassan yesy</v>
+      </c>
+      <c r="C18" t="str">
+        <v>3043.00</v>
+      </c>
+      <c r="D18" t="str">
+        <v>AC-1</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -2292,26 +1960,25 @@
         <v>0</v>
       </c>
       <c r="AA18">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB18">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>76</v>
-      </c>
-      <c r="B19" t="s">
-        <v>77</v>
-      </c>
-      <c r="C19" t="s">
-        <v>78</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
+        <f>SUM(E18:AA18)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>03464540151</v>
+      </c>
+      <c r="B19" t="str">
+        <v>Hassssan Test</v>
+      </c>
+      <c r="C19" t="str">
+        <v>37008.00</v>
+      </c>
+      <c r="D19" t="str">
+        <v>AC-1</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -2380,26 +2047,25 @@
         <v>0</v>
       </c>
       <c r="AA19">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB19">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>79</v>
-      </c>
-      <c r="B20" t="s">
-        <v>80</v>
-      </c>
-      <c r="C20" t="s">
-        <v>81</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
+        <f>SUM(E19:AA19)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>03333335599</v>
+      </c>
+      <c r="B20" t="str">
+        <v xml:space="preserve">restrict  pot </v>
+      </c>
+      <c r="C20" t="str">
+        <v>8730.50</v>
+      </c>
+      <c r="D20" t="str">
+        <v>AC-1</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -2468,26 +2134,25 @@
         <v>0</v>
       </c>
       <c r="AA20">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>82</v>
-      </c>
-      <c r="B21" t="s">
-        <v>83</v>
-      </c>
-      <c r="C21" t="s">
-        <v>40</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
+        <f>SUM(E20:AA20)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>03326299959</v>
+      </c>
+      <c r="B21" t="str">
+        <v>alfalaah test</v>
+      </c>
+      <c r="C21" t="str">
+        <v>5443.50</v>
+      </c>
+      <c r="D21" t="str">
+        <v>AC-1</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -2556,26 +2221,25 @@
         <v>0</v>
       </c>
       <c r="AA21">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB21">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>84</v>
-      </c>
-      <c r="B22" t="s">
-        <v>85</v>
-      </c>
-      <c r="C22" t="s">
-        <v>86</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
+        <f>SUM(E21:AA21)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>03564988457</v>
+      </c>
+      <c r="B22" t="str">
+        <v>test tsst</v>
+      </c>
+      <c r="C22" t="str">
+        <v>6798.00</v>
+      </c>
+      <c r="D22" t="str">
+        <v>AC-1</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -2644,26 +2308,25 @@
         <v>0</v>
       </c>
       <c r="AA22">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB22">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>87</v>
-      </c>
-      <c r="B23" t="s">
-        <v>88</v>
-      </c>
-      <c r="C23" t="s">
-        <v>89</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
+        <f>SUM(E22:AA22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>03464688000</v>
+      </c>
+      <c r="B23" t="str">
+        <v>yshsj hsyshs</v>
+      </c>
+      <c r="C23" t="str">
+        <v>2369.00</v>
+      </c>
+      <c r="D23" t="str">
+        <v>AC-1</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -2732,26 +2395,25 @@
         <v>0</v>
       </c>
       <c r="AA23">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB23">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>90</v>
-      </c>
-      <c r="B24" t="s">
-        <v>91</v>
-      </c>
-      <c r="C24" t="s">
-        <v>92</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
+        <f>SUM(E23:AA23)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>06735316616</v>
+      </c>
+      <c r="B24" t="str">
+        <v>test khan</v>
+      </c>
+      <c r="C24" t="str">
+        <v>1168.50</v>
+      </c>
+      <c r="D24" t="str">
+        <v>AC-1</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -2820,26 +2482,25 @@
         <v>0</v>
       </c>
       <c r="AA24">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB24">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>93</v>
-      </c>
-      <c r="B25" t="s">
-        <v>94</v>
-      </c>
-      <c r="C25" t="s">
-        <v>95</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
+        <f>SUM(E24:AA24)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>1234567890</v>
+      </c>
+      <c r="B25" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C25">
+        <v>1000000</v>
+      </c>
+      <c r="D25" t="str">
+        <v>AC-1</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -2908,18 +2569,1583 @@
         <v>0</v>
       </c>
       <c r="AA25">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB25">
-        <f t="shared" si="1"/>
+        <f>SUM(E25:AA25)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>1234567890</v>
+      </c>
+      <c r="B26" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C26">
+        <v>1000000</v>
+      </c>
+      <c r="D26" t="str">
+        <v>AC-1</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <v>0</v>
+      </c>
+      <c r="R26">
+        <v>0</v>
+      </c>
+      <c r="S26">
+        <v>0</v>
+      </c>
+      <c r="T26">
+        <v>0</v>
+      </c>
+      <c r="U26">
+        <v>0</v>
+      </c>
+      <c r="V26">
+        <v>0</v>
+      </c>
+      <c r="W26">
+        <v>0</v>
+      </c>
+      <c r="X26">
+        <v>0</v>
+      </c>
+      <c r="Y26">
+        <v>0</v>
+      </c>
+      <c r="Z26">
+        <v>0</v>
+      </c>
+      <c r="AA26">
+        <v>0</v>
+      </c>
+      <c r="AB26">
+        <f>SUM(E25:AA25)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>1234567890</v>
+      </c>
+      <c r="B27" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C27">
+        <v>1000000</v>
+      </c>
+      <c r="D27" t="str">
+        <v>AC-1</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <v>0</v>
+      </c>
+      <c r="R27">
+        <v>0</v>
+      </c>
+      <c r="S27">
+        <v>0</v>
+      </c>
+      <c r="T27">
+        <v>0</v>
+      </c>
+      <c r="U27">
+        <v>0</v>
+      </c>
+      <c r="V27">
+        <v>0</v>
+      </c>
+      <c r="W27">
+        <v>0</v>
+      </c>
+      <c r="X27">
+        <v>0</v>
+      </c>
+      <c r="Y27">
+        <v>0</v>
+      </c>
+      <c r="Z27">
+        <v>0</v>
+      </c>
+      <c r="AA27">
+        <v>0</v>
+      </c>
+      <c r="AB27">
+        <f>SUM(E25:AA25)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>1234567890</v>
+      </c>
+      <c r="B28" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C28">
+        <v>1000000</v>
+      </c>
+      <c r="D28" t="str">
+        <v>AC-1</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="P28">
+        <v>0</v>
+      </c>
+      <c r="Q28">
+        <v>0</v>
+      </c>
+      <c r="R28">
+        <v>0</v>
+      </c>
+      <c r="S28">
+        <v>0</v>
+      </c>
+      <c r="T28">
+        <v>0</v>
+      </c>
+      <c r="U28">
+        <v>0</v>
+      </c>
+      <c r="V28">
+        <v>0</v>
+      </c>
+      <c r="W28">
+        <v>0</v>
+      </c>
+      <c r="X28">
+        <v>0</v>
+      </c>
+      <c r="Y28">
+        <v>0</v>
+      </c>
+      <c r="Z28">
+        <v>0</v>
+      </c>
+      <c r="AA28">
+        <v>0</v>
+      </c>
+      <c r="AB28">
+        <f>SUM(E25:AA25)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>1234567890</v>
+      </c>
+      <c r="B29" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C29">
+        <v>1000000</v>
+      </c>
+      <c r="D29" t="str">
+        <v>AC-1</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <v>0</v>
+      </c>
+      <c r="N29">
+        <v>0</v>
+      </c>
+      <c r="O29">
+        <v>0</v>
+      </c>
+      <c r="P29">
+        <v>0</v>
+      </c>
+      <c r="Q29">
+        <v>0</v>
+      </c>
+      <c r="R29">
+        <v>0</v>
+      </c>
+      <c r="S29">
+        <v>0</v>
+      </c>
+      <c r="T29">
+        <v>0</v>
+      </c>
+      <c r="U29">
+        <v>0</v>
+      </c>
+      <c r="V29">
+        <v>0</v>
+      </c>
+      <c r="W29">
+        <v>0</v>
+      </c>
+      <c r="X29">
+        <v>0</v>
+      </c>
+      <c r="Y29">
+        <v>0</v>
+      </c>
+      <c r="Z29">
+        <v>0</v>
+      </c>
+      <c r="AA29">
+        <v>0</v>
+      </c>
+      <c r="AB29">
+        <f>SUM(E25:AA25)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>1234567890</v>
+      </c>
+      <c r="B30" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C30">
+        <v>1000000</v>
+      </c>
+      <c r="D30" t="str">
+        <v>AC-1</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <v>0</v>
+      </c>
+      <c r="N30">
+        <v>0</v>
+      </c>
+      <c r="O30">
+        <v>0</v>
+      </c>
+      <c r="P30">
+        <v>0</v>
+      </c>
+      <c r="Q30">
+        <v>0</v>
+      </c>
+      <c r="R30">
+        <v>0</v>
+      </c>
+      <c r="S30">
+        <v>0</v>
+      </c>
+      <c r="T30">
+        <v>0</v>
+      </c>
+      <c r="U30">
+        <v>0</v>
+      </c>
+      <c r="V30">
+        <v>0</v>
+      </c>
+      <c r="W30">
+        <v>0</v>
+      </c>
+      <c r="X30">
+        <v>0</v>
+      </c>
+      <c r="Y30">
+        <v>0</v>
+      </c>
+      <c r="Z30">
+        <v>0</v>
+      </c>
+      <c r="AA30">
+        <v>0</v>
+      </c>
+      <c r="AB30">
+        <f>SUM(E25:AA25)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>1234567890</v>
+      </c>
+      <c r="B31" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C31">
+        <v>1000000</v>
+      </c>
+      <c r="D31" t="str">
+        <v>AC-1</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <v>0</v>
+      </c>
+      <c r="O31">
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <v>0</v>
+      </c>
+      <c r="Q31">
+        <v>0</v>
+      </c>
+      <c r="R31">
+        <v>0</v>
+      </c>
+      <c r="S31">
+        <v>0</v>
+      </c>
+      <c r="T31">
+        <v>0</v>
+      </c>
+      <c r="U31">
+        <v>0</v>
+      </c>
+      <c r="V31">
+        <v>0</v>
+      </c>
+      <c r="W31">
+        <v>0</v>
+      </c>
+      <c r="X31">
+        <v>0</v>
+      </c>
+      <c r="Y31">
+        <v>0</v>
+      </c>
+      <c r="Z31">
+        <v>0</v>
+      </c>
+      <c r="AA31">
+        <v>0</v>
+      </c>
+      <c r="AB31">
+        <f>SUM(E25:AA25)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>1234567890</v>
+      </c>
+      <c r="B32" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C32">
+        <v>1000000</v>
+      </c>
+      <c r="D32" t="str">
+        <v>AC-1</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
+      <c r="N32">
+        <v>0</v>
+      </c>
+      <c r="O32">
+        <v>0</v>
+      </c>
+      <c r="P32">
+        <v>0</v>
+      </c>
+      <c r="Q32">
+        <v>0</v>
+      </c>
+      <c r="R32">
+        <v>0</v>
+      </c>
+      <c r="S32">
+        <v>0</v>
+      </c>
+      <c r="T32">
+        <v>0</v>
+      </c>
+      <c r="U32">
+        <v>0</v>
+      </c>
+      <c r="V32">
+        <v>0</v>
+      </c>
+      <c r="W32">
+        <v>0</v>
+      </c>
+      <c r="X32">
+        <v>0</v>
+      </c>
+      <c r="Y32">
+        <v>0</v>
+      </c>
+      <c r="Z32">
+        <v>0</v>
+      </c>
+      <c r="AA32">
+        <v>0</v>
+      </c>
+      <c r="AB32">
+        <f>SUM(E25:AA25)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>1234567890</v>
+      </c>
+      <c r="B33" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C33">
+        <v>1000000</v>
+      </c>
+      <c r="D33" t="str">
+        <v>AC-1</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+      <c r="M33">
+        <v>0</v>
+      </c>
+      <c r="N33">
+        <v>0</v>
+      </c>
+      <c r="O33">
+        <v>0</v>
+      </c>
+      <c r="P33">
+        <v>0</v>
+      </c>
+      <c r="Q33">
+        <v>0</v>
+      </c>
+      <c r="R33">
+        <v>0</v>
+      </c>
+      <c r="S33">
+        <v>0</v>
+      </c>
+      <c r="T33">
+        <v>0</v>
+      </c>
+      <c r="U33">
+        <v>0</v>
+      </c>
+      <c r="V33">
+        <v>0</v>
+      </c>
+      <c r="W33">
+        <v>0</v>
+      </c>
+      <c r="X33">
+        <v>0</v>
+      </c>
+      <c r="Y33">
+        <v>0</v>
+      </c>
+      <c r="Z33">
+        <v>0</v>
+      </c>
+      <c r="AA33">
+        <v>0</v>
+      </c>
+      <c r="AB33">
+        <f>SUM(E25:AA25)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>1234567890</v>
+      </c>
+      <c r="B34" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C34">
+        <v>1000000</v>
+      </c>
+      <c r="D34" t="str">
+        <v>AC-1</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <v>0</v>
+      </c>
+      <c r="L34">
+        <v>0</v>
+      </c>
+      <c r="M34">
+        <v>0</v>
+      </c>
+      <c r="N34">
+        <v>0</v>
+      </c>
+      <c r="O34">
+        <v>0</v>
+      </c>
+      <c r="P34">
+        <v>0</v>
+      </c>
+      <c r="Q34">
+        <v>0</v>
+      </c>
+      <c r="R34">
+        <v>0</v>
+      </c>
+      <c r="S34">
+        <v>0</v>
+      </c>
+      <c r="T34">
+        <v>0</v>
+      </c>
+      <c r="U34">
+        <v>0</v>
+      </c>
+      <c r="V34">
+        <v>0</v>
+      </c>
+      <c r="W34">
+        <v>0</v>
+      </c>
+      <c r="X34">
+        <v>0</v>
+      </c>
+      <c r="Y34">
+        <v>0</v>
+      </c>
+      <c r="Z34">
+        <v>0</v>
+      </c>
+      <c r="AA34">
+        <v>0</v>
+      </c>
+      <c r="AB34">
+        <f>SUM(E25:AA25)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>1234567890</v>
+      </c>
+      <c r="B35" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C35">
+        <v>1000000</v>
+      </c>
+      <c r="D35" t="str">
+        <v>AC-1</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <v>0</v>
+      </c>
+      <c r="O35">
+        <v>0</v>
+      </c>
+      <c r="P35">
+        <v>0</v>
+      </c>
+      <c r="Q35">
+        <v>0</v>
+      </c>
+      <c r="R35">
+        <v>0</v>
+      </c>
+      <c r="S35">
+        <v>0</v>
+      </c>
+      <c r="T35">
+        <v>0</v>
+      </c>
+      <c r="U35">
+        <v>0</v>
+      </c>
+      <c r="V35">
+        <v>0</v>
+      </c>
+      <c r="W35">
+        <v>0</v>
+      </c>
+      <c r="X35">
+        <v>0</v>
+      </c>
+      <c r="Y35">
+        <v>0</v>
+      </c>
+      <c r="Z35">
+        <v>0</v>
+      </c>
+      <c r="AA35">
+        <v>0</v>
+      </c>
+      <c r="AB35">
+        <f>SUM(E25:AA25)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>1234567890</v>
+      </c>
+      <c r="B36" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C36">
+        <v>1000000</v>
+      </c>
+      <c r="D36" t="str">
+        <v>AC-1</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
+      <c r="L36">
+        <v>0</v>
+      </c>
+      <c r="M36">
+        <v>0</v>
+      </c>
+      <c r="N36">
+        <v>0</v>
+      </c>
+      <c r="O36">
+        <v>0</v>
+      </c>
+      <c r="P36">
+        <v>0</v>
+      </c>
+      <c r="Q36">
+        <v>0</v>
+      </c>
+      <c r="R36">
+        <v>0</v>
+      </c>
+      <c r="S36">
+        <v>0</v>
+      </c>
+      <c r="T36">
+        <v>0</v>
+      </c>
+      <c r="U36">
+        <v>0</v>
+      </c>
+      <c r="V36">
+        <v>0</v>
+      </c>
+      <c r="W36">
+        <v>0</v>
+      </c>
+      <c r="X36">
+        <v>0</v>
+      </c>
+      <c r="Y36">
+        <v>0</v>
+      </c>
+      <c r="Z36">
+        <v>0</v>
+      </c>
+      <c r="AA36">
+        <v>0</v>
+      </c>
+      <c r="AB36">
+        <f>SUM(E25:AA25)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>1234567890</v>
+      </c>
+      <c r="B37" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C37">
+        <v>1000000</v>
+      </c>
+      <c r="D37" t="str">
+        <v>AC-1</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <v>0</v>
+      </c>
+      <c r="L37">
+        <v>0</v>
+      </c>
+      <c r="M37">
+        <v>0</v>
+      </c>
+      <c r="N37">
+        <v>0</v>
+      </c>
+      <c r="O37">
+        <v>0</v>
+      </c>
+      <c r="P37">
+        <v>0</v>
+      </c>
+      <c r="Q37">
+        <v>0</v>
+      </c>
+      <c r="R37">
+        <v>0</v>
+      </c>
+      <c r="S37">
+        <v>0</v>
+      </c>
+      <c r="T37">
+        <v>0</v>
+      </c>
+      <c r="U37">
+        <v>0</v>
+      </c>
+      <c r="V37">
+        <v>0</v>
+      </c>
+      <c r="W37">
+        <v>0</v>
+      </c>
+      <c r="X37">
+        <v>0</v>
+      </c>
+      <c r="Y37">
+        <v>0</v>
+      </c>
+      <c r="Z37">
+        <v>0</v>
+      </c>
+      <c r="AA37">
+        <v>0</v>
+      </c>
+      <c r="AB37">
+        <f>SUM(E25:AA25)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>1234567890</v>
+      </c>
+      <c r="B38" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C38">
+        <v>1000000</v>
+      </c>
+      <c r="D38" t="str">
+        <v>AC-1</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+      <c r="K38">
+        <v>0</v>
+      </c>
+      <c r="L38">
+        <v>0</v>
+      </c>
+      <c r="M38">
+        <v>0</v>
+      </c>
+      <c r="N38">
+        <v>0</v>
+      </c>
+      <c r="O38">
+        <v>0</v>
+      </c>
+      <c r="P38">
+        <v>0</v>
+      </c>
+      <c r="Q38">
+        <v>0</v>
+      </c>
+      <c r="R38">
+        <v>0</v>
+      </c>
+      <c r="S38">
+        <v>0</v>
+      </c>
+      <c r="T38">
+        <v>0</v>
+      </c>
+      <c r="U38">
+        <v>0</v>
+      </c>
+      <c r="V38">
+        <v>0</v>
+      </c>
+      <c r="W38">
+        <v>0</v>
+      </c>
+      <c r="X38">
+        <v>0</v>
+      </c>
+      <c r="Y38">
+        <v>0</v>
+      </c>
+      <c r="Z38">
+        <v>0</v>
+      </c>
+      <c r="AA38">
+        <v>0</v>
+      </c>
+      <c r="AB38">
+        <f>SUM(E25:AA25)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>1234567890</v>
+      </c>
+      <c r="B39" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C39">
+        <v>1000000</v>
+      </c>
+      <c r="D39" t="str">
+        <v>AC-2</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <v>0</v>
+      </c>
+      <c r="K39">
+        <v>0</v>
+      </c>
+      <c r="L39">
+        <v>0</v>
+      </c>
+      <c r="M39">
+        <v>0</v>
+      </c>
+      <c r="N39">
+        <v>0</v>
+      </c>
+      <c r="O39">
+        <v>0</v>
+      </c>
+      <c r="P39">
+        <v>0</v>
+      </c>
+      <c r="Q39">
+        <v>0</v>
+      </c>
+      <c r="R39">
+        <v>0</v>
+      </c>
+      <c r="S39">
+        <v>0</v>
+      </c>
+      <c r="T39">
+        <v>0</v>
+      </c>
+      <c r="U39">
+        <v>0</v>
+      </c>
+      <c r="V39">
+        <v>0</v>
+      </c>
+      <c r="W39">
+        <v>0</v>
+      </c>
+      <c r="X39">
+        <v>0</v>
+      </c>
+      <c r="Y39">
+        <v>0</v>
+      </c>
+      <c r="Z39">
+        <v>0</v>
+      </c>
+      <c r="AA39">
+        <v>0</v>
+      </c>
+      <c r="AB39">
+        <f>SUM(E25:AA25)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>1234567890</v>
+      </c>
+      <c r="B40" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C40">
+        <v>1000000</v>
+      </c>
+      <c r="D40" t="str">
+        <v>AC-3</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
+      <c r="L40">
+        <v>0</v>
+      </c>
+      <c r="M40">
+        <v>0</v>
+      </c>
+      <c r="N40">
+        <v>0</v>
+      </c>
+      <c r="O40">
+        <v>0</v>
+      </c>
+      <c r="P40">
+        <v>0</v>
+      </c>
+      <c r="Q40">
+        <v>0</v>
+      </c>
+      <c r="R40">
+        <v>0</v>
+      </c>
+      <c r="S40">
+        <v>0</v>
+      </c>
+      <c r="T40">
+        <v>0</v>
+      </c>
+      <c r="U40">
+        <v>0</v>
+      </c>
+      <c r="V40">
+        <v>0</v>
+      </c>
+      <c r="W40">
+        <v>0</v>
+      </c>
+      <c r="X40">
+        <v>0</v>
+      </c>
+      <c r="Y40">
+        <v>0</v>
+      </c>
+      <c r="Z40">
+        <v>0</v>
+      </c>
+      <c r="AA40">
+        <v>0</v>
+      </c>
+      <c r="AB40">
+        <f>SUM(E25:AA25)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>1234567890</v>
+      </c>
+      <c r="B41" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C41">
+        <v>1000000</v>
+      </c>
+      <c r="D41" t="str">
+        <v>AC-4</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <v>0</v>
+      </c>
+      <c r="L41">
+        <v>0</v>
+      </c>
+      <c r="M41">
+        <v>0</v>
+      </c>
+      <c r="N41">
+        <v>0</v>
+      </c>
+      <c r="O41">
+        <v>0</v>
+      </c>
+      <c r="P41">
+        <v>0</v>
+      </c>
+      <c r="Q41">
+        <v>0</v>
+      </c>
+      <c r="R41">
+        <v>0</v>
+      </c>
+      <c r="S41">
+        <v>0</v>
+      </c>
+      <c r="T41">
+        <v>0</v>
+      </c>
+      <c r="U41">
+        <v>0</v>
+      </c>
+      <c r="V41">
+        <v>0</v>
+      </c>
+      <c r="W41">
+        <v>0</v>
+      </c>
+      <c r="X41">
+        <v>0</v>
+      </c>
+      <c r="Y41">
+        <v>0</v>
+      </c>
+      <c r="Z41">
+        <v>0</v>
+      </c>
+      <c r="AA41">
+        <v>0</v>
+      </c>
+      <c r="AB41">
+        <f>SUM(E25:AA25)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>1234567890</v>
+      </c>
+      <c r="B42" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C42">
+        <v>1000000</v>
+      </c>
+      <c r="D42" t="str">
+        <v>AC-1</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+      <c r="K42">
+        <v>0</v>
+      </c>
+      <c r="L42">
+        <v>0</v>
+      </c>
+      <c r="M42">
+        <v>0</v>
+      </c>
+      <c r="N42">
+        <v>0</v>
+      </c>
+      <c r="O42">
+        <v>0</v>
+      </c>
+      <c r="P42">
+        <v>0</v>
+      </c>
+      <c r="Q42">
+        <v>0</v>
+      </c>
+      <c r="R42">
+        <v>0</v>
+      </c>
+      <c r="S42">
+        <v>0</v>
+      </c>
+      <c r="T42">
+        <v>0</v>
+      </c>
+      <c r="U42">
+        <v>0</v>
+      </c>
+      <c r="V42">
+        <v>0</v>
+      </c>
+      <c r="W42">
+        <v>0</v>
+      </c>
+      <c r="X42">
+        <v>0</v>
+      </c>
+      <c r="Y42">
+        <v>0</v>
+      </c>
+      <c r="Z42">
+        <v>0</v>
+      </c>
+      <c r="AA42">
+        <v>0</v>
+      </c>
+      <c r="AB42">
+        <f>SUM(E25:AA25)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>1234567890</v>
+      </c>
+      <c r="B43" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C43">
+        <v>1000000</v>
+      </c>
+      <c r="D43" t="str">
+        <v>AC-2</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <v>0</v>
+      </c>
+      <c r="L43">
+        <v>0</v>
+      </c>
+      <c r="M43">
+        <v>0</v>
+      </c>
+      <c r="N43">
+        <v>0</v>
+      </c>
+      <c r="O43">
+        <v>0</v>
+      </c>
+      <c r="P43">
+        <v>0</v>
+      </c>
+      <c r="Q43">
+        <v>0</v>
+      </c>
+      <c r="R43">
+        <v>0</v>
+      </c>
+      <c r="S43">
+        <v>0</v>
+      </c>
+      <c r="T43">
+        <v>0</v>
+      </c>
+      <c r="U43">
+        <v>0</v>
+      </c>
+      <c r="V43">
+        <v>0</v>
+      </c>
+      <c r="W43">
+        <v>0</v>
+      </c>
+      <c r="X43">
+        <v>0</v>
+      </c>
+      <c r="Y43">
+        <v>0</v>
+      </c>
+      <c r="Z43">
+        <v>0</v>
+      </c>
+      <c r="AA43">
+        <v>0</v>
+      </c>
+      <c r="AB43">
+        <f>SUM(E25:AA25)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:Z1 A3:Z25 A2:D2 F2:Z2" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AB44"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>